<commit_message>
fix: improve Project Euler 6 presentation
</commit_message>
<xml_diff>
--- a/Project Euler 006.xlsx
+++ b/Project Euler 006.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8536EC04-B4FD-4C86-B329-40B50A56C99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDA5D35-006A-4F34-9408-1EAFA9436EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9FE02216-42E7-4B55-B329-98B67CF9EEFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>First 100 natural numbers</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>&lt;-- answer</t>
+  </si>
+  <si>
+    <t>Project Euler 6: Sum Square Difference</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,930 +436,935 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD01C019-ADCA-4890-92AA-2110727D0612}">
-  <dimension ref="C2:E104"/>
+  <dimension ref="B2:D106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="10.90625" style="1"/>
+    <col min="2" max="3" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="D2" s="2">
-        <f>SUM(C5:C104)^2-SUM(D5:D104)</f>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="2">
+        <f>SUM(B7:B106)^2-SUM(C7:C106)</f>
         <v>25164150</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="4" t="s">
+    <row r="6" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C5" s="1">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
-        <f>C5*C5</f>
+      <c r="C7" s="1">
+        <f>B7*B7</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C6" s="1">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" ref="D6:D69" si="0">C6*C6</f>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:C71" si="0">B8*B8</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C7" s="1">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C8" s="1">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="D8" s="1">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C9" s="1">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C10" s="1">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="D10" s="1">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C11" s="1">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
         <v>7</v>
       </c>
-      <c r="D11" s="1">
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C12" s="1">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
         <v>8</v>
       </c>
-      <c r="D12" s="1">
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C13" s="1">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="D13" s="1">
+      <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C14" s="1">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="D14" s="1">
+      <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C15" s="1">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="1">
         <v>11</v>
       </c>
-      <c r="D15" s="1">
+      <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="1">
         <v>12</v>
       </c>
-      <c r="D16" s="1">
+      <c r="C18" s="1">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="1">
         <v>13</v>
       </c>
-      <c r="D17" s="1">
+      <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="1">
         <v>14</v>
       </c>
-      <c r="D18" s="1">
+      <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C19" s="1">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="1">
         <v>15</v>
       </c>
-      <c r="D19" s="1">
+      <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C20" s="1">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="1">
         <v>16</v>
       </c>
-      <c r="D20" s="1">
+      <c r="C22" s="1">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C21" s="1">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="1">
         <v>17</v>
       </c>
-      <c r="D21" s="1">
+      <c r="C23" s="1">
         <f t="shared" si="0"/>
         <v>289</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C22" s="1">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
         <v>18</v>
       </c>
-      <c r="D22" s="1">
+      <c r="C24" s="1">
         <f t="shared" si="0"/>
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C23" s="1">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
         <v>19</v>
       </c>
-      <c r="D23" s="1">
+      <c r="C25" s="1">
         <f t="shared" si="0"/>
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C24" s="1">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
         <v>20</v>
       </c>
-      <c r="D24" s="1">
+      <c r="C26" s="1">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C25" s="1">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="1">
         <v>21</v>
       </c>
-      <c r="D25" s="1">
+      <c r="C27" s="1">
         <f t="shared" si="0"/>
         <v>441</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C26" s="1">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" s="1">
         <v>22</v>
       </c>
-      <c r="D26" s="1">
+      <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>484</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C27" s="1">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="1">
         <v>23</v>
       </c>
-      <c r="D27" s="1">
+      <c r="C29" s="1">
         <f t="shared" si="0"/>
         <v>529</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C28" s="1">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="1">
         <v>24</v>
       </c>
-      <c r="D28" s="1">
+      <c r="C30" s="1">
         <f t="shared" si="0"/>
         <v>576</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C29" s="1">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="1">
         <v>25</v>
       </c>
-      <c r="D29" s="1">
+      <c r="C31" s="1">
         <f t="shared" si="0"/>
         <v>625</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C30" s="1">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="1">
         <v>26</v>
       </c>
-      <c r="D30" s="1">
+      <c r="C32" s="1">
         <f t="shared" si="0"/>
         <v>676</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C31" s="1">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="1">
         <v>27</v>
       </c>
-      <c r="D31" s="1">
+      <c r="C33" s="1">
         <f t="shared" si="0"/>
         <v>729</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C32" s="1">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="1">
         <v>28</v>
       </c>
-      <c r="D32" s="1">
+      <c r="C34" s="1">
         <f t="shared" si="0"/>
         <v>784</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C33" s="1">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="1">
         <v>29</v>
       </c>
-      <c r="D33" s="1">
+      <c r="C35" s="1">
         <f t="shared" si="0"/>
         <v>841</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C34" s="1">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" s="1">
         <v>30</v>
       </c>
-      <c r="D34" s="1">
+      <c r="C36" s="1">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C35" s="1">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="1">
         <v>31</v>
       </c>
-      <c r="D35" s="1">
+      <c r="C37" s="1">
         <f t="shared" si="0"/>
         <v>961</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C36" s="1">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="1">
         <v>32</v>
       </c>
-      <c r="D36" s="1">
+      <c r="C38" s="1">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C37" s="1">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="1">
         <v>33</v>
       </c>
-      <c r="D37" s="1">
+      <c r="C39" s="1">
         <f t="shared" si="0"/>
         <v>1089</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C38" s="1">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="1">
         <v>34</v>
       </c>
-      <c r="D38" s="1">
+      <c r="C40" s="1">
         <f t="shared" si="0"/>
         <v>1156</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C39" s="1">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="1">
         <v>35</v>
       </c>
-      <c r="D39" s="1">
+      <c r="C41" s="1">
         <f t="shared" si="0"/>
         <v>1225</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C40" s="1">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="1">
         <v>36</v>
       </c>
-      <c r="D40" s="1">
+      <c r="C42" s="1">
         <f t="shared" si="0"/>
         <v>1296</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C41" s="1">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" s="1">
         <v>37</v>
       </c>
-      <c r="D41" s="1">
+      <c r="C43" s="1">
         <f t="shared" si="0"/>
         <v>1369</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C42" s="1">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" s="1">
         <v>38</v>
       </c>
-      <c r="D42" s="1">
+      <c r="C44" s="1">
         <f t="shared" si="0"/>
         <v>1444</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C43" s="1">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" s="1">
         <v>39</v>
       </c>
-      <c r="D43" s="1">
+      <c r="C45" s="1">
         <f t="shared" si="0"/>
         <v>1521</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C44" s="1">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" s="1">
         <v>40</v>
       </c>
-      <c r="D44" s="1">
+      <c r="C46" s="1">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C45" s="1">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" s="1">
         <v>41</v>
       </c>
-      <c r="D45" s="1">
+      <c r="C47" s="1">
         <f t="shared" si="0"/>
         <v>1681</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C46" s="1">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="1">
         <v>42</v>
       </c>
-      <c r="D46" s="1">
+      <c r="C48" s="1">
         <f t="shared" si="0"/>
         <v>1764</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C47" s="1">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" s="1">
         <v>43</v>
       </c>
-      <c r="D47" s="1">
+      <c r="C49" s="1">
         <f t="shared" si="0"/>
         <v>1849</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C48" s="1">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" s="1">
         <v>44</v>
       </c>
-      <c r="D48" s="1">
+      <c r="C50" s="1">
         <f t="shared" si="0"/>
         <v>1936</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C49" s="1">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" s="1">
         <v>45</v>
       </c>
-      <c r="D49" s="1">
+      <c r="C51" s="1">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C50" s="1">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" s="1">
         <v>46</v>
       </c>
-      <c r="D50" s="1">
+      <c r="C52" s="1">
         <f t="shared" si="0"/>
         <v>2116</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C51" s="1">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" s="1">
         <v>47</v>
       </c>
-      <c r="D51" s="1">
+      <c r="C53" s="1">
         <f t="shared" si="0"/>
         <v>2209</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C52" s="1">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="1">
         <v>48</v>
       </c>
-      <c r="D52" s="1">
+      <c r="C54" s="1">
         <f t="shared" si="0"/>
         <v>2304</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C53" s="1">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="1">
         <v>49</v>
       </c>
-      <c r="D53" s="1">
+      <c r="C55" s="1">
         <f t="shared" si="0"/>
         <v>2401</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C54" s="1">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="1">
         <v>50</v>
       </c>
-      <c r="D54" s="1">
+      <c r="C56" s="1">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C55" s="1">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" s="1">
         <v>51</v>
       </c>
-      <c r="D55" s="1">
+      <c r="C57" s="1">
         <f t="shared" si="0"/>
         <v>2601</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C56" s="1">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" s="1">
         <v>52</v>
       </c>
-      <c r="D56" s="1">
+      <c r="C58" s="1">
         <f t="shared" si="0"/>
         <v>2704</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C57" s="1">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" s="1">
         <v>53</v>
       </c>
-      <c r="D57" s="1">
+      <c r="C59" s="1">
         <f t="shared" si="0"/>
         <v>2809</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C58" s="1">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" s="1">
         <v>54</v>
       </c>
-      <c r="D58" s="1">
+      <c r="C60" s="1">
         <f t="shared" si="0"/>
         <v>2916</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C59" s="1">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="1">
         <v>55</v>
       </c>
-      <c r="D59" s="1">
+      <c r="C61" s="1">
         <f t="shared" si="0"/>
         <v>3025</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C60" s="1">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="1">
         <v>56</v>
       </c>
-      <c r="D60" s="1">
+      <c r="C62" s="1">
         <f t="shared" si="0"/>
         <v>3136</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C61" s="1">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63" s="1">
         <v>57</v>
       </c>
-      <c r="D61" s="1">
+      <c r="C63" s="1">
         <f t="shared" si="0"/>
         <v>3249</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C62" s="1">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B64" s="1">
         <v>58</v>
       </c>
-      <c r="D62" s="1">
+      <c r="C64" s="1">
         <f t="shared" si="0"/>
         <v>3364</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C63" s="1">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B65" s="1">
         <v>59</v>
       </c>
-      <c r="D63" s="1">
+      <c r="C65" s="1">
         <f t="shared" si="0"/>
         <v>3481</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C64" s="1">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66" s="1">
         <v>60</v>
       </c>
-      <c r="D64" s="1">
+      <c r="C66" s="1">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C65" s="1">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67" s="1">
         <v>61</v>
       </c>
-      <c r="D65" s="1">
+      <c r="C67" s="1">
         <f t="shared" si="0"/>
         <v>3721</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C66" s="1">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68" s="1">
         <v>62</v>
       </c>
-      <c r="D66" s="1">
+      <c r="C68" s="1">
         <f t="shared" si="0"/>
         <v>3844</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C67" s="1">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69" s="1">
         <v>63</v>
       </c>
-      <c r="D67" s="1">
+      <c r="C69" s="1">
         <f t="shared" si="0"/>
         <v>3969</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C68" s="1">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70" s="1">
         <v>64</v>
       </c>
-      <c r="D68" s="1">
+      <c r="C70" s="1">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C69" s="1">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B71" s="1">
         <v>65</v>
       </c>
-      <c r="D69" s="1">
+      <c r="C71" s="1">
         <f t="shared" si="0"/>
         <v>4225</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C70" s="1">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B72" s="1">
         <v>66</v>
       </c>
-      <c r="D70" s="1">
-        <f t="shared" ref="D70:D104" si="1">C70*C70</f>
+      <c r="C72" s="1">
+        <f t="shared" ref="C72:C106" si="1">B72*B72</f>
         <v>4356</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C71" s="1">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73" s="1">
         <v>67</v>
       </c>
-      <c r="D71" s="1">
+      <c r="C73" s="1">
         <f t="shared" si="1"/>
         <v>4489</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C72" s="1">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74" s="1">
         <v>68</v>
       </c>
-      <c r="D72" s="1">
+      <c r="C74" s="1">
         <f t="shared" si="1"/>
         <v>4624</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C73" s="1">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B75" s="1">
         <v>69</v>
       </c>
-      <c r="D73" s="1">
+      <c r="C75" s="1">
         <f t="shared" si="1"/>
         <v>4761</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C74" s="1">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B76" s="1">
         <v>70</v>
       </c>
-      <c r="D74" s="1">
+      <c r="C76" s="1">
         <f t="shared" si="1"/>
         <v>4900</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C75" s="1">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B77" s="1">
         <v>71</v>
       </c>
-      <c r="D75" s="1">
+      <c r="C77" s="1">
         <f t="shared" si="1"/>
         <v>5041</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C76" s="1">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B78" s="1">
         <v>72</v>
       </c>
-      <c r="D76" s="1">
+      <c r="C78" s="1">
         <f t="shared" si="1"/>
         <v>5184</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C77" s="1">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B79" s="1">
         <v>73</v>
       </c>
-      <c r="D77" s="1">
+      <c r="C79" s="1">
         <f t="shared" si="1"/>
         <v>5329</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C78" s="1">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B80" s="1">
         <v>74</v>
       </c>
-      <c r="D78" s="1">
+      <c r="C80" s="1">
         <f t="shared" si="1"/>
         <v>5476</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C79" s="1">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B81" s="1">
         <v>75</v>
       </c>
-      <c r="D79" s="1">
+      <c r="C81" s="1">
         <f t="shared" si="1"/>
         <v>5625</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C80" s="1">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B82" s="1">
         <v>76</v>
       </c>
-      <c r="D80" s="1">
+      <c r="C82" s="1">
         <f t="shared" si="1"/>
         <v>5776</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C81" s="1">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B83" s="1">
         <v>77</v>
       </c>
-      <c r="D81" s="1">
+      <c r="C83" s="1">
         <f t="shared" si="1"/>
         <v>5929</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C82" s="1">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B84" s="1">
         <v>78</v>
       </c>
-      <c r="D82" s="1">
+      <c r="C84" s="1">
         <f t="shared" si="1"/>
         <v>6084</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C83" s="1">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B85" s="1">
         <v>79</v>
       </c>
-      <c r="D83" s="1">
+      <c r="C85" s="1">
         <f t="shared" si="1"/>
         <v>6241</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C84" s="1">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B86" s="1">
         <v>80</v>
       </c>
-      <c r="D84" s="1">
+      <c r="C86" s="1">
         <f t="shared" si="1"/>
         <v>6400</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C85" s="1">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B87" s="1">
         <v>81</v>
       </c>
-      <c r="D85" s="1">
+      <c r="C87" s="1">
         <f t="shared" si="1"/>
         <v>6561</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C86" s="1">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B88" s="1">
         <v>82</v>
       </c>
-      <c r="D86" s="1">
+      <c r="C88" s="1">
         <f t="shared" si="1"/>
         <v>6724</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C87" s="1">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B89" s="1">
         <v>83</v>
       </c>
-      <c r="D87" s="1">
+      <c r="C89" s="1">
         <f t="shared" si="1"/>
         <v>6889</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C88" s="1">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B90" s="1">
         <v>84</v>
       </c>
-      <c r="D88" s="1">
+      <c r="C90" s="1">
         <f t="shared" si="1"/>
         <v>7056</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C89" s="1">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B91" s="1">
         <v>85</v>
       </c>
-      <c r="D89" s="1">
+      <c r="C91" s="1">
         <f t="shared" si="1"/>
         <v>7225</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C90" s="1">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B92" s="1">
         <v>86</v>
       </c>
-      <c r="D90" s="1">
+      <c r="C92" s="1">
         <f t="shared" si="1"/>
         <v>7396</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C91" s="1">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B93" s="1">
         <v>87</v>
       </c>
-      <c r="D91" s="1">
+      <c r="C93" s="1">
         <f t="shared" si="1"/>
         <v>7569</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C92" s="1">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B94" s="1">
         <v>88</v>
       </c>
-      <c r="D92" s="1">
+      <c r="C94" s="1">
         <f t="shared" si="1"/>
         <v>7744</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C93" s="1">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B95" s="1">
         <v>89</v>
       </c>
-      <c r="D93" s="1">
+      <c r="C95" s="1">
         <f t="shared" si="1"/>
         <v>7921</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C94" s="1">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B96" s="1">
         <v>90</v>
       </c>
-      <c r="D94" s="1">
+      <c r="C96" s="1">
         <f t="shared" si="1"/>
         <v>8100</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C95" s="1">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B97" s="1">
         <v>91</v>
       </c>
-      <c r="D95" s="1">
+      <c r="C97" s="1">
         <f t="shared" si="1"/>
         <v>8281</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C96" s="1">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B98" s="1">
         <v>92</v>
       </c>
-      <c r="D96" s="1">
+      <c r="C98" s="1">
         <f t="shared" si="1"/>
         <v>8464</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C97" s="1">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B99" s="1">
         <v>93</v>
       </c>
-      <c r="D97" s="1">
+      <c r="C99" s="1">
         <f t="shared" si="1"/>
         <v>8649</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C98" s="1">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B100" s="1">
         <v>94</v>
       </c>
-      <c r="D98" s="1">
+      <c r="C100" s="1">
         <f t="shared" si="1"/>
         <v>8836</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C99" s="1">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B101" s="1">
         <v>95</v>
       </c>
-      <c r="D99" s="1">
+      <c r="C101" s="1">
         <f t="shared" si="1"/>
         <v>9025</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C100" s="1">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B102" s="1">
         <v>96</v>
       </c>
-      <c r="D100" s="1">
+      <c r="C102" s="1">
         <f t="shared" si="1"/>
         <v>9216</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C101" s="1">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B103" s="1">
         <v>97</v>
       </c>
-      <c r="D101" s="1">
+      <c r="C103" s="1">
         <f t="shared" si="1"/>
         <v>9409</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C102" s="1">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B104" s="1">
         <v>98</v>
       </c>
-      <c r="D102" s="1">
+      <c r="C104" s="1">
         <f t="shared" si="1"/>
         <v>9604</v>
       </c>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C103" s="1">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B105" s="1">
         <v>99</v>
       </c>
-      <c r="D103" s="1">
+      <c r="C105" s="1">
         <f t="shared" si="1"/>
         <v>9801</v>
       </c>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C104" s="1">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B106" s="1">
         <v>100</v>
       </c>
-      <c r="D104" s="1">
+      <c r="C106" s="1">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>

</xml_diff>

<commit_message>
fix: improve Project Euler 6
</commit_message>
<xml_diff>
--- a/Project Euler 006.xlsx
+++ b/Project Euler 006.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDA5D35-006A-4F34-9408-1EAFA9436EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD132BDB-6C42-43C2-9D79-73EB6E2C125F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9FE02216-42E7-4B55-B329-98B67CF9EEFD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9FE02216-42E7-4B55-B329-98B67CF9EEFD}"/>
   </bookViews>
   <sheets>
-    <sheet name="PE 006" sheetId="1" r:id="rId1"/>
+    <sheet name="PE 006 A" sheetId="1" r:id="rId1"/>
+    <sheet name="PE 006 B" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>First 100 natural numbers</t>
   </si>
@@ -48,6 +71,9 @@
   </si>
   <si>
     <t>Project Euler 6: Sum Square Difference</t>
+  </si>
+  <si>
+    <t>with array formulas</t>
   </si>
 </sst>
 </file>
@@ -74,15 +100,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,16 +122,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD01C019-ADCA-4890-92AA-2110727D0612}">
   <dimension ref="B2:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,909 +510,909 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <f>B7*B7</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <f t="shared" ref="C8:C71" si="0">B8*B8</f>
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="1">
+      <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="1">
+      <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
+      <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>169</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="1">
+      <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <f t="shared" si="0"/>
         <v>196</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="1">
+      <c r="B21" s="4">
         <v>15</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="1">
+      <c r="B22" s="4">
         <v>16</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="1">
+      <c r="B23" s="4">
         <v>17</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <f t="shared" si="0"/>
         <v>289</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="1">
+      <c r="B24" s="4">
         <v>18</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>324</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="1">
+      <c r="B25" s="4">
         <v>19</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <f t="shared" si="0"/>
         <v>361</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="1">
+      <c r="B26" s="4">
         <v>20</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="1">
+      <c r="B27" s="4">
         <v>21</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>441</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="1">
+      <c r="B28" s="4">
         <v>22</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="4">
         <f t="shared" si="0"/>
         <v>484</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="1">
+      <c r="B29" s="4">
         <v>23</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <f t="shared" si="0"/>
         <v>529</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="1">
+      <c r="B30" s="4">
         <v>24</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="4">
         <f t="shared" si="0"/>
         <v>576</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="1">
+      <c r="B31" s="4">
         <v>25</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="4">
         <f t="shared" si="0"/>
         <v>625</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="1">
+      <c r="B32" s="4">
         <v>26</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="4">
         <f t="shared" si="0"/>
         <v>676</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="1">
+      <c r="B33" s="4">
         <v>27</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="4">
         <f t="shared" si="0"/>
         <v>729</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="1">
+      <c r="B34" s="4">
         <v>28</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="4">
         <f t="shared" si="0"/>
         <v>784</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="1">
+      <c r="B35" s="4">
         <v>29</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="4">
         <f t="shared" si="0"/>
         <v>841</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="1">
+      <c r="B36" s="4">
         <v>30</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="4">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="1">
+      <c r="B37" s="4">
         <v>31</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="4">
         <f t="shared" si="0"/>
         <v>961</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="1">
+      <c r="B38" s="4">
         <v>32</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="4">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="1">
+      <c r="B39" s="4">
         <v>33</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="4">
         <f t="shared" si="0"/>
         <v>1089</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="1">
+      <c r="B40" s="4">
         <v>34</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="4">
         <f t="shared" si="0"/>
         <v>1156</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="1">
+      <c r="B41" s="4">
         <v>35</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="4">
         <f t="shared" si="0"/>
         <v>1225</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="1">
+      <c r="B42" s="4">
         <v>36</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="4">
         <f t="shared" si="0"/>
         <v>1296</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="1">
+      <c r="B43" s="4">
         <v>37</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="4">
         <f t="shared" si="0"/>
         <v>1369</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="1">
+      <c r="B44" s="4">
         <v>38</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="4">
         <f t="shared" si="0"/>
         <v>1444</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="1">
+      <c r="B45" s="4">
         <v>39</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="4">
         <f t="shared" si="0"/>
         <v>1521</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="1">
+      <c r="B46" s="4">
         <v>40</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="4">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="1">
+      <c r="B47" s="4">
         <v>41</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="4">
         <f t="shared" si="0"/>
         <v>1681</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="1">
+      <c r="B48" s="4">
         <v>42</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="4">
         <f t="shared" si="0"/>
         <v>1764</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="1">
+      <c r="B49" s="4">
         <v>43</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="4">
         <f t="shared" si="0"/>
         <v>1849</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="1">
+      <c r="B50" s="4">
         <v>44</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="4">
         <f t="shared" si="0"/>
         <v>1936</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="1">
+      <c r="B51" s="4">
         <v>45</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="4">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="1">
+      <c r="B52" s="4">
         <v>46</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="4">
         <f t="shared" si="0"/>
         <v>2116</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="1">
+      <c r="B53" s="4">
         <v>47</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="4">
         <f t="shared" si="0"/>
         <v>2209</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="1">
+      <c r="B54" s="4">
         <v>48</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="4">
         <f t="shared" si="0"/>
         <v>2304</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="1">
+      <c r="B55" s="4">
         <v>49</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="4">
         <f t="shared" si="0"/>
         <v>2401</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="1">
+      <c r="B56" s="4">
         <v>50</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="4">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="1">
+      <c r="B57" s="4">
         <v>51</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="4">
         <f t="shared" si="0"/>
         <v>2601</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="1">
+      <c r="B58" s="4">
         <v>52</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="4">
         <f t="shared" si="0"/>
         <v>2704</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="1">
+      <c r="B59" s="4">
         <v>53</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="4">
         <f t="shared" si="0"/>
         <v>2809</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="1">
+      <c r="B60" s="4">
         <v>54</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="4">
         <f t="shared" si="0"/>
         <v>2916</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="1">
+      <c r="B61" s="4">
         <v>55</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="4">
         <f t="shared" si="0"/>
         <v>3025</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="1">
+      <c r="B62" s="4">
         <v>56</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="4">
         <f t="shared" si="0"/>
         <v>3136</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="1">
+      <c r="B63" s="4">
         <v>57</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="4">
         <f t="shared" si="0"/>
         <v>3249</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64" s="1">
+      <c r="B64" s="4">
         <v>58</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="4">
         <f t="shared" si="0"/>
         <v>3364</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B65" s="1">
+      <c r="B65" s="4">
         <v>59</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="4">
         <f t="shared" si="0"/>
         <v>3481</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B66" s="1">
+      <c r="B66" s="4">
         <v>60</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="4">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B67" s="1">
+      <c r="B67" s="4">
         <v>61</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="4">
         <f t="shared" si="0"/>
         <v>3721</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="1">
+      <c r="B68" s="4">
         <v>62</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="4">
         <f t="shared" si="0"/>
         <v>3844</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69" s="1">
+      <c r="B69" s="4">
         <v>63</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="4">
         <f t="shared" si="0"/>
         <v>3969</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="1">
+      <c r="B70" s="4">
         <v>64</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="4">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="1">
+      <c r="B71" s="4">
         <v>65</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" s="4">
         <f t="shared" si="0"/>
         <v>4225</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="1">
+      <c r="B72" s="4">
         <v>66</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="4">
         <f t="shared" ref="C72:C106" si="1">B72*B72</f>
         <v>4356</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="1">
+      <c r="B73" s="4">
         <v>67</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="4">
         <f t="shared" si="1"/>
         <v>4489</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="1">
+      <c r="B74" s="4">
         <v>68</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" s="4">
         <f t="shared" si="1"/>
         <v>4624</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="1">
+      <c r="B75" s="4">
         <v>69</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="4">
         <f t="shared" si="1"/>
         <v>4761</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76" s="1">
+      <c r="B76" s="4">
         <v>70</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="4">
         <f t="shared" si="1"/>
         <v>4900</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="1">
+      <c r="B77" s="4">
         <v>71</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="4">
         <f t="shared" si="1"/>
         <v>5041</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="1">
+      <c r="B78" s="4">
         <v>72</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="4">
         <f t="shared" si="1"/>
         <v>5184</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="1">
+      <c r="B79" s="4">
         <v>73</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="4">
         <f t="shared" si="1"/>
         <v>5329</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B80" s="1">
+      <c r="B80" s="4">
         <v>74</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="4">
         <f t="shared" si="1"/>
         <v>5476</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="1">
+      <c r="B81" s="4">
         <v>75</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="4">
         <f t="shared" si="1"/>
         <v>5625</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82" s="1">
+      <c r="B82" s="4">
         <v>76</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="4">
         <f t="shared" si="1"/>
         <v>5776</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="1">
+      <c r="B83" s="4">
         <v>77</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="4">
         <f t="shared" si="1"/>
         <v>5929</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84" s="1">
+      <c r="B84" s="4">
         <v>78</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" s="4">
         <f t="shared" si="1"/>
         <v>6084</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85" s="1">
+      <c r="B85" s="4">
         <v>79</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="4">
         <f t="shared" si="1"/>
         <v>6241</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86" s="1">
+      <c r="B86" s="4">
         <v>80</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="4">
         <f t="shared" si="1"/>
         <v>6400</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="1">
+      <c r="B87" s="4">
         <v>81</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="4">
         <f t="shared" si="1"/>
         <v>6561</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B88" s="1">
+      <c r="B88" s="4">
         <v>82</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" s="4">
         <f t="shared" si="1"/>
         <v>6724</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89" s="1">
+      <c r="B89" s="4">
         <v>83</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" s="4">
         <f t="shared" si="1"/>
         <v>6889</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B90" s="1">
+      <c r="B90" s="4">
         <v>84</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="4">
         <f t="shared" si="1"/>
         <v>7056</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B91" s="1">
+      <c r="B91" s="4">
         <v>85</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="4">
         <f t="shared" si="1"/>
         <v>7225</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B92" s="1">
+      <c r="B92" s="4">
         <v>86</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92" s="4">
         <f t="shared" si="1"/>
         <v>7396</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B93" s="1">
+      <c r="B93" s="4">
         <v>87</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93" s="4">
         <f t="shared" si="1"/>
         <v>7569</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="1">
+      <c r="B94" s="4">
         <v>88</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="4">
         <f t="shared" si="1"/>
         <v>7744</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="1">
+      <c r="B95" s="4">
         <v>89</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="4">
         <f t="shared" si="1"/>
         <v>7921</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96" s="1">
+      <c r="B96" s="4">
         <v>90</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="4">
         <f t="shared" si="1"/>
         <v>8100</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="1">
+      <c r="B97" s="4">
         <v>91</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="4">
         <f t="shared" si="1"/>
         <v>8281</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98" s="1">
+      <c r="B98" s="4">
         <v>92</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="4">
         <f t="shared" si="1"/>
         <v>8464</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99" s="1">
+      <c r="B99" s="4">
         <v>93</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="4">
         <f t="shared" si="1"/>
         <v>8649</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B100" s="1">
+      <c r="B100" s="4">
         <v>94</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100" s="4">
         <f t="shared" si="1"/>
         <v>8836</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B101" s="1">
+      <c r="B101" s="4">
         <v>95</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="4">
         <f t="shared" si="1"/>
         <v>9025</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B102" s="1">
+      <c r="B102" s="4">
         <v>96</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C102" s="4">
         <f t="shared" si="1"/>
         <v>9216</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B103" s="1">
+      <c r="B103" s="4">
         <v>97</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103" s="4">
         <f t="shared" si="1"/>
         <v>9409</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B104" s="1">
+      <c r="B104" s="4">
         <v>98</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C104" s="4">
         <f t="shared" si="1"/>
         <v>9604</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B105" s="1">
+      <c r="B105" s="4">
         <v>99</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="4">
         <f t="shared" si="1"/>
         <v>9801</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="1">
+      <c r="B106" s="4">
         <v>100</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C106" s="4">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
@@ -1373,4 +1421,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C76321-34CA-4615-B81D-4105BFB6DD8F}">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" cm="1">
+        <f t="array" ref="B5">SUM( _xlfn.SEQUENCE(100) )^2
+      - SUM( _xlfn.MAP(_xlfn.SEQUENCE(100), _xlfn.LAMBDA(_xlpm.a,_xlpm.a^2)) )</f>
+        <v>25164150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add explanations to 'Project Euler 6' section of README
</commit_message>
<xml_diff>
--- a/Project Euler 006.xlsx
+++ b/Project Euler 006.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D556B9-9FF7-4CD9-959F-A04EA0CD23CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F25A1-BF75-49C7-8D90-F177D51DF5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9FE02216-42E7-4B55-B329-98B67CF9EEFD}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>First 100 natural numbers</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>2) Using spreadsheet capabilities</t>
+  </si>
+  <si>
+    <t>https://projecteuler.net/problem=6</t>
+  </si>
+  <si>
+    <t>for 10:</t>
+  </si>
+  <si>
+    <t>for 100:</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +129,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -161,6 +176,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -184,15 +207,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>28122</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>156029</xdr:rowOff>
+      <xdr:colOff>9072</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3629</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>432708</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>36798</xdr:rowOff>
+      <xdr:colOff>299358</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68548</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -215,7 +238,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="637722" y="524329"/>
+          <a:off x="618672" y="740229"/>
           <a:ext cx="5617936" cy="1538119"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -229,7 +252,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -545,991 +568,1021 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C76321-34CA-4615-B81D-4105BFB6DD8F}">
-  <dimension ref="B2:D121"/>
+  <dimension ref="B2:F124"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C15" s="2" cm="1">
-        <f t="array" ref="C15">SUM( _xlfn.SEQUENCE(100) )^2
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="9">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C17" s="8" cm="1">
+        <f t="array" ref="C17">SUM( _xlfn.SEQUENCE(C16) )^2
+      - SUM( _xlfn.MAP(_xlfn.SEQUENCE(C16), _xlfn.LAMBDA(_xlpm.a,_xlpm.a^2)) )</f>
+        <v>2640</v>
+      </c>
+      <c r="E17" s="2" cm="1">
+        <f t="array" ref="E17">SUM( _xlfn.SEQUENCE(100) )^2
       - SUM( _xlfn.MAP(_xlfn.SEQUENCE(100), _xlfn.LAMBDA(_xlpm.a,_xlpm.a^2)) )</f>
         <v>25164150</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="1"/>
-      <c r="C19" s="2">
-        <f>SUM(B22:B121)^2-SUM(C22:C121)</f>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
+        <f>SUM(B25:B34)^2-SUM(C25:C34)</f>
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2">
+        <f>SUM(B25:B124)^2-SUM(C25:C124)</f>
         <v>25164150</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="7" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="4">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="4">
-        <f>B22*B22</f>
+      <c r="C25" s="4">
+        <f>B25*B25</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="4">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="4">
-        <f t="shared" ref="C23:C86" si="0">B23*B23</f>
+      <c r="C26" s="4">
+        <f t="shared" ref="C26:C89" si="0">B26*B26</f>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="4">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
         <v>3</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="4">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
         <v>4</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C28" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="4">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
         <v>5</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C29" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="4">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
         <v>6</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C30" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="4">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
         <v>7</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C31" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="4">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
         <v>8</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C32" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="4">
-        <v>9</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="4">
-        <v>10</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="4">
-        <v>11</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" si="0"/>
-        <v>121</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="0"/>
-        <v>169</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="0"/>
-        <v>289</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="0"/>
-        <v>361</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="0"/>
-        <v>441</v>
+        <v>324</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="0"/>
-        <v>484</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="4">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="0"/>
-        <v>529</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="4">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="0"/>
-        <v>576</v>
+        <v>441</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="0"/>
-        <v>625</v>
+        <v>484</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="4">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="0"/>
-        <v>676</v>
+        <v>529</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="4">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="0"/>
-        <v>729</v>
+        <v>576</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="4">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="0"/>
-        <v>784</v>
+        <v>625</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="0"/>
-        <v>841</v>
+        <v>676</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>729</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C52" s="4">
         <f t="shared" si="0"/>
-        <v>961</v>
+        <v>784</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="4">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" si="0"/>
-        <v>1024</v>
+        <v>841</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="4">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" si="0"/>
-        <v>1089</v>
+        <v>900</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="4">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="0"/>
-        <v>1156</v>
+        <v>961</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="4">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="0"/>
-        <v>1225</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="4">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="0"/>
-        <v>1296</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="4">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="0"/>
-        <v>1369</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="4">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C59" s="4">
         <f t="shared" si="0"/>
-        <v>1444</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="4">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C60" s="4">
         <f t="shared" si="0"/>
-        <v>1521</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="4">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C61" s="4">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="4">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C62" s="4">
         <f t="shared" si="0"/>
-        <v>1681</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="4">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C63" s="4">
         <f t="shared" si="0"/>
-        <v>1764</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="4">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C64" s="4">
         <f t="shared" si="0"/>
-        <v>1849</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="4">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C65" s="4">
         <f t="shared" si="0"/>
-        <v>1936</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="4">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C66" s="4">
         <f t="shared" si="0"/>
-        <v>2025</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="4">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C67" s="4">
         <f t="shared" si="0"/>
-        <v>2116</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="4">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C68" s="4">
         <f t="shared" si="0"/>
-        <v>2209</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="4">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C69" s="4">
         <f t="shared" si="0"/>
-        <v>2304</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="4">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C70" s="4">
         <f t="shared" si="0"/>
-        <v>2401</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="4">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C71" s="4">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="4">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C72" s="4">
         <f t="shared" si="0"/>
-        <v>2601</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="4">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C73" s="4">
         <f t="shared" si="0"/>
-        <v>2704</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="4">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C74" s="4">
         <f t="shared" si="0"/>
-        <v>2809</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" s="4">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C75" s="4">
         <f t="shared" si="0"/>
-        <v>2916</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="4">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C76" s="4">
         <f t="shared" si="0"/>
-        <v>3025</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="4">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C77" s="4">
         <f t="shared" si="0"/>
-        <v>3136</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="4">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C78" s="4">
         <f t="shared" si="0"/>
-        <v>3249</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="4">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C79" s="4">
         <f t="shared" si="0"/>
-        <v>3364</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="4">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C80" s="4">
         <f t="shared" si="0"/>
-        <v>3481</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="4">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C81" s="4">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="4">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C82" s="4">
         <f t="shared" si="0"/>
-        <v>3721</v>
+        <v>3364</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="4">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C83" s="4">
         <f t="shared" si="0"/>
-        <v>3844</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="4">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C84" s="4">
         <f t="shared" si="0"/>
-        <v>3969</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="4">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C85" s="4">
         <f t="shared" si="0"/>
-        <v>4096</v>
+        <v>3721</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="4">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C86" s="4">
         <f t="shared" si="0"/>
-        <v>4225</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="4">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C87" s="4">
-        <f t="shared" ref="C87:C121" si="1">B87*B87</f>
-        <v>4356</v>
+        <f t="shared" si="0"/>
+        <v>3969</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="4">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C88" s="4">
-        <f t="shared" si="1"/>
-        <v>4489</v>
+        <f t="shared" si="0"/>
+        <v>4096</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="4">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C89" s="4">
-        <f t="shared" si="1"/>
-        <v>4624</v>
+        <f t="shared" si="0"/>
+        <v>4225</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="4">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C90" s="4">
-        <f t="shared" si="1"/>
-        <v>4761</v>
+        <f t="shared" ref="C90:C124" si="1">B90*B90</f>
+        <v>4356</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C91" s="4">
         <f t="shared" si="1"/>
-        <v>4900</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="4">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C92" s="4">
         <f t="shared" si="1"/>
-        <v>5041</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="4">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C93" s="4">
         <f t="shared" si="1"/>
-        <v>5184</v>
+        <v>4761</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" s="4">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C94" s="4">
         <f t="shared" si="1"/>
-        <v>5329</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" s="4">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C95" s="4">
         <f t="shared" si="1"/>
-        <v>5476</v>
+        <v>5041</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" s="4">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C96" s="4">
         <f t="shared" si="1"/>
-        <v>5625</v>
+        <v>5184</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="4">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C97" s="4">
         <f t="shared" si="1"/>
-        <v>5776</v>
+        <v>5329</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" s="4">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C98" s="4">
         <f t="shared" si="1"/>
-        <v>5929</v>
+        <v>5476</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="4">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C99" s="4">
         <f t="shared" si="1"/>
-        <v>6084</v>
+        <v>5625</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100" s="4">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C100" s="4">
         <f t="shared" si="1"/>
-        <v>6241</v>
+        <v>5776</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101" s="4">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C101" s="4">
         <f t="shared" si="1"/>
-        <v>6400</v>
+        <v>5929</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102" s="4">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C102" s="4">
         <f t="shared" si="1"/>
-        <v>6561</v>
+        <v>6084</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103" s="4">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C103" s="4">
         <f t="shared" si="1"/>
-        <v>6724</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="4">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C104" s="4">
         <f t="shared" si="1"/>
-        <v>6889</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105" s="4">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C105" s="4">
         <f t="shared" si="1"/>
-        <v>7056</v>
+        <v>6561</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106" s="4">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C106" s="4">
         <f t="shared" si="1"/>
-        <v>7225</v>
+        <v>6724</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="4">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C107" s="4">
         <f t="shared" si="1"/>
-        <v>7396</v>
+        <v>6889</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108" s="4">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C108" s="4">
         <f t="shared" si="1"/>
-        <v>7569</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109" s="4">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C109" s="4">
         <f t="shared" si="1"/>
-        <v>7744</v>
+        <v>7225</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110" s="4">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C110" s="4">
         <f t="shared" si="1"/>
-        <v>7921</v>
+        <v>7396</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111" s="4">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C111" s="4">
         <f t="shared" si="1"/>
-        <v>8100</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112" s="4">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C112" s="4">
         <f t="shared" si="1"/>
-        <v>8281</v>
+        <v>7744</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113" s="4">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C113" s="4">
         <f t="shared" si="1"/>
-        <v>8464</v>
+        <v>7921</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114" s="4">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C114" s="4">
         <f t="shared" si="1"/>
-        <v>8649</v>
+        <v>8100</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115" s="4">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C115" s="4">
         <f t="shared" si="1"/>
-        <v>8836</v>
+        <v>8281</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116" s="4">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C116" s="4">
         <f t="shared" si="1"/>
-        <v>9025</v>
+        <v>8464</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117" s="4">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C117" s="4">
         <f t="shared" si="1"/>
-        <v>9216</v>
+        <v>8649</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118" s="4">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C118" s="4">
         <f t="shared" si="1"/>
-        <v>9409</v>
+        <v>8836</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119" s="4">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C119" s="4">
         <f t="shared" si="1"/>
-        <v>9604</v>
+        <v>9025</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120" s="4">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C120" s="4">
         <f t="shared" si="1"/>
-        <v>9801</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B121" s="4">
+        <v>97</v>
+      </c>
+      <c r="C121" s="4">
+        <f t="shared" si="1"/>
+        <v>9409</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B122" s="4">
+        <v>98</v>
+      </c>
+      <c r="C122" s="4">
+        <f t="shared" si="1"/>
+        <v>9604</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B123" s="4">
+        <v>99</v>
+      </c>
+      <c r="C123" s="4">
+        <f t="shared" si="1"/>
+        <v>9801</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B124" s="4">
         <v>100</v>
       </c>
-      <c r="C121" s="4">
+      <c r="C124" s="4">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>

</xml_diff>